<commit_message>
Einarbeitung der neuen Diagramme
</commit_message>
<xml_diff>
--- a/Fingeruntersuchung.xlsx
+++ b/Fingeruntersuchung.xlsx
@@ -359,10 +359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,6 +507,40 @@
         <v>103.75</v>
       </c>
     </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <f>B$7 / 1.45 * 5</f>
+        <v>275</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:I9" si="0">C$7 / 1.45 * 5</f>
+        <v>380.17241379310349</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>428.44827586206895</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>288.79310344827587</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>373.27586206896558</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>357.75862068965517</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>